<commit_message>
fixed the gerbers and BOM file for the xiao version
</commit_message>
<xml_diff>
--- a/tiny20/xiao/Tiny20BOM.xlsx
+++ b/tiny20/xiao/Tiny20BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enzoc\Documents\GitHub\Tiny20\tiny20\xiao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F111DB51-A831-4CFA-8856-AA80D6D5E931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE94B19-5C2A-4596-B42A-CC9546BC4839}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10290" yWindow="1770" windowWidth="14205" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="2985" windowWidth="17325" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tiny20BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Designator</t>
   </si>
@@ -71,6 +71,27 @@
   </si>
   <si>
     <t>Battery_Cell</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/33029465106.html</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/4000917776872.html</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/1005001308084552.html</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/4000685483225.html</t>
+  </si>
+  <si>
+    <t>https://es.aliexpress.com/item/32959996455.html</t>
+  </si>
+  <si>
+    <t>1 pack = 10u</t>
+  </si>
+  <si>
+    <t>do not solder</t>
   </si>
 </sst>
 </file>
@@ -911,15 +932,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -943,8 +964,14 @@
       <c r="C2">
         <v>10</v>
       </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -954,8 +981,14 @@
       <c r="C3">
         <v>2</v>
       </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -968,8 +1001,11 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -979,8 +1015,14 @@
       <c r="C5">
         <v>1</v>
       </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -990,8 +1032,14 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1000,6 +1048,12 @@
       </c>
       <c r="C7">
         <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>